<commit_message>
TraceMap Review beendet Version 1.5
</commit_message>
<xml_diff>
--- a/Pflichtenheft/Tracemap/TracabilityMap.xlsx
+++ b/Pflichtenheft/Tracemap/TracabilityMap.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="88">
   <si>
     <t>Anforderungen</t>
   </si>
@@ -185,24 +185,6 @@
     <t>1-4, 14, 15</t>
   </si>
   <si>
-    <t>16-26,</t>
-  </si>
-  <si>
-    <t>1-4, 5-10, 13, 27-34</t>
-  </si>
-  <si>
-    <t>1-4,  5-10, 11-13,27-34</t>
-  </si>
-  <si>
-    <t>11,12,21, 22, 25-34</t>
-  </si>
-  <si>
-    <t>5-12, 16-20, 31-34,</t>
-  </si>
-  <si>
-    <t>5-12, 21-24 31-34,</t>
-  </si>
-  <si>
     <t>16-26</t>
   </si>
   <si>
@@ -260,24 +242,12 @@
     <t>1.1, 1.2</t>
   </si>
   <si>
-    <t xml:space="preserve">1.1, 1.2, 2.6-2.8, 3, 4, 5-7, 8.1, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.1, 1.2, 2.1-2.5, 3, 4, 4.1, 5-7, 8.2, </t>
-  </si>
-  <si>
     <t>1.3, 1.4, 9.1, 9.2, 10-14</t>
   </si>
   <si>
     <t>1.1, 1.2, 2.1-2.8, 3, 4,  4.1, 8.1,8.2, 9.1, 9.2, 10, 11</t>
   </si>
   <si>
-    <t>1.1, 1.2, 5, 8.1,8.2, 11, 12</t>
-  </si>
-  <si>
-    <t>1.1, 1.2, 6, 7, 8.1,8.2, 13, 14</t>
-  </si>
-  <si>
     <t>9.2, 10-14</t>
   </si>
   <si>
@@ -294,6 +264,42 @@
   </si>
   <si>
     <t>Review (Änderungen Akzeptanztests)</t>
+  </si>
+  <si>
+    <t>Review (Änderungen Systemtest)</t>
+  </si>
+  <si>
+    <t>1.5</t>
+  </si>
+  <si>
+    <t>1.4.1</t>
+  </si>
+  <si>
+    <t>5-12,21, 22, 25-34</t>
+  </si>
+  <si>
+    <t>11,12, 21-24, 31-34, 39-42</t>
+  </si>
+  <si>
+    <t>1-4, 5-10, 13, 27-42</t>
+  </si>
+  <si>
+    <t>1-4,  5-10, 11-13,27-43</t>
+  </si>
+  <si>
+    <t>5-12, 16-20, 35-38</t>
+  </si>
+  <si>
+    <t>1.1, 1.2, 2.6-2.8, 3, 4, 5-7, 8.1</t>
+  </si>
+  <si>
+    <t>1.1, 1.2, 2.1-2.5, 3, 4, 4.1, 5-7, 8.2</t>
+  </si>
+  <si>
+    <t>1.1, 1.2, 6, 7, 8.1, 8.2, 13, 14</t>
+  </si>
+  <si>
+    <t>1.1, 1.2, 5, 8.1, 8.2, 11, 12</t>
   </si>
 </sst>
 </file>
@@ -435,7 +441,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -463,20 +468,25 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -795,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A29" sqref="A29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -804,7 +814,7 @@
     <col min="1" max="1" width="24.140625" customWidth="1"/>
     <col min="2" max="2" width="23.28515625" customWidth="1"/>
     <col min="3" max="3" width="27.140625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="5" customWidth="1"/>
     <col min="5" max="5" width="30" style="5" customWidth="1"/>
     <col min="6" max="6" width="21.42578125" style="5" customWidth="1"/>
   </cols>
@@ -822,290 +832,292 @@
       <c r="D1" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="E1" s="9" t="s">
+      <c r="E1" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="9" t="s">
-        <v>72</v>
+      <c r="F1" s="8" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="14"/>
+      <c r="B2" s="10"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="13"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="12"/>
-      <c r="D3" s="11" t="s">
+      <c r="C3" s="11"/>
+      <c r="D3" s="21" t="s">
         <v>48</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>81</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F4" s="13" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>82</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="13" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="F6" s="13" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" s="10"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="12"/>
+      <c r="F7" s="13"/>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D8" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="22" t="s">
+        <v>58</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="D9" s="21" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="22"/>
+      <c r="F9" s="13" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="D10" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="22"/>
+      <c r="F10" s="13" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>28</v>
+      </c>
+      <c r="C12" s="11"/>
+      <c r="D12" s="15">
+        <v>43</v>
+      </c>
+      <c r="E12" s="12" t="s">
         <v>60</v>
       </c>
-      <c r="F3" s="14" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" s="11" t="s">
+      <c r="F12" s="13" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="10"/>
+      <c r="C13" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="D13" s="21" t="s">
+        <v>49</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="F13" s="13"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="B14" s="10"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="12"/>
+      <c r="F14" s="13"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" s="10"/>
+      <c r="C15" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F15" s="13"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" s="10"/>
+      <c r="C16" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F16" s="13"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="10"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="12" t="s">
+        <v>64</v>
+      </c>
+      <c r="F17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="10"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="F18" s="13"/>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="E4" s="13" t="s">
-        <v>84</v>
-      </c>
-      <c r="F4" s="14" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="14" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F6" s="14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B7" s="11"/>
-      <c r="C7" s="12"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>52</v>
-      </c>
-      <c r="E8" s="25" t="s">
-        <v>64</v>
-      </c>
-      <c r="F8" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="11" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="25"/>
-      <c r="F9" s="14" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" s="11" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>53</v>
-      </c>
-      <c r="E10" s="25"/>
-      <c r="F10" s="14" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11" s="11" t="s">
-        <v>27</v>
-      </c>
-      <c r="C11" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" s="11"/>
-      <c r="E11" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="F11" s="14" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="C12" s="12"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="F12" s="14" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="11"/>
-      <c r="C13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>55</v>
-      </c>
-      <c r="E13" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="F13" s="14"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="11"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="14"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D15" s="11"/>
-      <c r="E15" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="14"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16" s="11"/>
-      <c r="C16" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="D16" s="11"/>
-      <c r="E16" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="F16" s="14"/>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="13" t="s">
-        <v>70</v>
-      </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18" s="11"/>
-      <c r="C18" s="12"/>
-      <c r="D18" s="11"/>
-      <c r="E18" s="16" t="s">
+      <c r="B19" s="10"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F18" s="14"/>
-    </row>
-    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="15" t="s">
-        <v>56</v>
-      </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="12"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="F19" s="14"/>
+      <c r="F19" s="13"/>
     </row>
     <row r="22" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="2" t="s">
@@ -1125,105 +1137,113 @@
       </c>
     </row>
     <row r="24" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="19" t="s">
+      <c r="A24" s="18" t="s">
         <v>42</v>
       </c>
-      <c r="B24" s="21"/>
-      <c r="C24" s="17" t="s">
+      <c r="B24" s="19"/>
+      <c r="C24" s="16" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="19" t="s">
+      <c r="A25" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B25" s="21">
+      <c r="B25" s="19">
         <v>43081</v>
       </c>
-      <c r="C25" s="17" t="s">
-        <v>59</v>
+      <c r="C25" s="16" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="19" t="s">
-        <v>57</v>
-      </c>
-      <c r="B26" s="18">
+      <c r="A26" s="18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B26" s="17">
         <v>43082</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="16" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="21">
+      <c r="A27" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B27" s="19">
         <v>43083</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="20"/>
+      <c r="D27" s="25"/>
     </row>
     <row r="28" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="B28" s="21">
+      <c r="A28" s="18" t="s">
+        <v>72</v>
+      </c>
+      <c r="B28" s="19">
         <v>43089</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>83</v>
+      <c r="C28" s="16" t="s">
+        <v>73</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="B29" s="21">
+      <c r="A29" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B29" s="19">
         <v>43112</v>
       </c>
-      <c r="C29" s="17"/>
-    </row>
-    <row r="30" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="19"/>
-      <c r="B30" s="21"/>
-      <c r="C30" s="17"/>
+      <c r="C29" s="16" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" s="19">
+        <v>43114</v>
+      </c>
+      <c r="C30" s="16" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="19"/>
-      <c r="B31" s="21"/>
-      <c r="C31" s="17"/>
+      <c r="A31" s="18"/>
+      <c r="B31" s="19"/>
+      <c r="C31" s="16"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A32" s="22"/>
+      <c r="A32" s="20"/>
       <c r="B32" s="23"/>
       <c r="C32" s="24"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="22"/>
+      <c r="A33" s="20"/>
       <c r="B33" s="23"/>
       <c r="C33" s="24"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="22"/>
+      <c r="A34" s="20"/>
       <c r="B34" s="23"/>
       <c r="C34" s="24"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="22"/>
+      <c r="A35" s="20"/>
       <c r="B35" s="23"/>
       <c r="C35" s="24"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="22"/>
+      <c r="A36" s="20"/>
       <c r="B36" s="23"/>
       <c r="C36" s="24"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="22"/>
+      <c r="A37" s="20"/>
       <c r="B37" s="23"/>
       <c r="C37" s="24"/>
     </row>

</xml_diff>

<commit_message>
Akzeptanztest and TraceMap modified
</commit_message>
<xml_diff>
--- a/Pflichtenheft/Tracemap/TracabilityMap.xlsx
+++ b/Pflichtenheft/Tracemap/TracabilityMap.xlsx
@@ -209,18 +209,9 @@
     <t>1.6-1.8, 4.1, 4.2, 5.1, 5.2, 7.1, 15.1, 16.1</t>
   </si>
   <si>
-    <t>1.1-1.5, 2.1, 8.1, 8.2, 9.2, 10.3, 11.3, 12.2, 13.1, 13.2, 14.1</t>
-  </si>
-  <si>
-    <t>1.1-1.5, 2.1, 2.2, 8.1, 8.2, 9.1, 9.2, 10.1-10.3, 11.1-11.3, 12.1, 12.2, 13.1, 13.2, 14.1</t>
-  </si>
-  <si>
     <t>6.1</t>
   </si>
   <si>
-    <t>8.1, 8.2, 10.1-10.3, 11.1-11.3</t>
-  </si>
-  <si>
     <t>4.1, 5.1, 5.2, 7.1, 15.1</t>
   </si>
   <si>
@@ -230,9 +221,6 @@
     <t>1.6-1.8, 7.1</t>
   </si>
   <si>
-    <t>2.1, 2.2</t>
-  </si>
-  <si>
     <t>13.1, 13.2</t>
   </si>
   <si>
@@ -300,6 +288,18 @@
   </si>
   <si>
     <t>1.1, 1.2, 5, 8.1, 8.2, 11, 12</t>
+  </si>
+  <si>
+    <t>1.1-1.5, 2.1, 8.1, 8.2, 9.2, 10.3, 10.4, 11.3, 12.2, 13.1, 13.2, 14.1</t>
+  </si>
+  <si>
+    <t>1.1-1.5, 2.1, 2.2, 8.1, 8.2, 9.1, 9.2, 10.1-10.4, 11.1-11.3, 12.1, 12.2, 13.1, 13.2, 14.1</t>
+  </si>
+  <si>
+    <t>8.1, 8.2, 10.1-10.4, 11.1-11.3</t>
+  </si>
+  <si>
+    <t>2.1, 2.2, 10.4</t>
   </si>
 </sst>
 </file>
@@ -477,6 +477,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -485,9 +488,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,8 +805,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -836,7 +836,7 @@
         <v>47</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,7 +864,7 @@
         <v>54</v>
       </c>
       <c r="F3" s="13" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -878,13 +878,13 @@
         <v>31</v>
       </c>
       <c r="D4" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="E4" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>81</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F4" s="13" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -898,13 +898,13 @@
         <v>30</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E5" s="12" t="s">
-        <v>57</v>
+        <v>84</v>
       </c>
       <c r="F5" s="13" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -924,7 +924,7 @@
         <v>56</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -948,13 +948,13 @@
         <v>32</v>
       </c>
       <c r="D8" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="22" t="s">
-        <v>58</v>
+        <v>75</v>
+      </c>
+      <c r="E8" s="23" t="s">
+        <v>85</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
@@ -968,11 +968,11 @@
         <v>33</v>
       </c>
       <c r="D9" s="21" t="s">
-        <v>80</v>
-      </c>
-      <c r="E9" s="22"/>
+        <v>76</v>
+      </c>
+      <c r="E9" s="23"/>
       <c r="F9" s="13" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="45" x14ac:dyDescent="0.25">
@@ -986,11 +986,11 @@
         <v>34</v>
       </c>
       <c r="D10" s="21" t="s">
-        <v>83</v>
-      </c>
-      <c r="E10" s="22"/>
+        <v>79</v>
+      </c>
+      <c r="E10" s="23"/>
       <c r="F10" s="13" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -1008,7 +1008,7 @@
         <v>55</v>
       </c>
       <c r="F11" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -1023,10 +1023,10 @@
         <v>43</v>
       </c>
       <c r="E12" s="12" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="F12" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,7 +1041,7 @@
         <v>49</v>
       </c>
       <c r="E13" s="12" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="F13" s="13"/>
     </row>
@@ -1065,7 +1065,7 @@
       </c>
       <c r="D15" s="21"/>
       <c r="E15" s="12" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="F15" s="13"/>
     </row>
@@ -1079,7 +1079,7 @@
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="12" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="F16" s="13"/>
     </row>
@@ -1091,7 +1091,7 @@
       <c r="C17" s="11"/>
       <c r="D17" s="21"/>
       <c r="E17" s="12" t="s">
-        <v>64</v>
+        <v>87</v>
       </c>
       <c r="F17" s="13"/>
     </row>
@@ -1103,7 +1103,7 @@
       <c r="C18" s="11"/>
       <c r="D18" s="21"/>
       <c r="E18" s="15" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F18" s="13"/>
     </row>
@@ -1115,7 +1115,7 @@
       <c r="C19" s="11"/>
       <c r="D19" s="21"/>
       <c r="E19" s="12" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="F19" s="13"/>
     </row>
@@ -1177,39 +1177,39 @@
       <c r="C27" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="D27" s="25"/>
+      <c r="D27" s="22"/>
     </row>
     <row r="28" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="18" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B28" s="19">
         <v>43089</v>
       </c>
       <c r="C28" s="16" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="B29" s="19">
         <v>43112</v>
       </c>
       <c r="C29" s="16" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="B30" s="19">
         <v>43114</v>
       </c>
       <c r="C30" s="16" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1219,33 +1219,33 @@
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
-      <c r="B32" s="23"/>
-      <c r="C32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="25"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
-      <c r="B33" s="23"/>
-      <c r="C33" s="24"/>
+      <c r="B33" s="24"/>
+      <c r="C33" s="25"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
-      <c r="B34" s="23"/>
-      <c r="C34" s="24"/>
+      <c r="B34" s="24"/>
+      <c r="C34" s="25"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
-      <c r="B35" s="23"/>
-      <c r="C35" s="24"/>
+      <c r="B35" s="24"/>
+      <c r="C35" s="25"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
-      <c r="B36" s="23"/>
-      <c r="C36" s="24"/>
+      <c r="B36" s="24"/>
+      <c r="C36" s="25"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="20"/>
-      <c r="B37" s="23"/>
-      <c r="C37" s="24"/>
+      <c r="B37" s="24"/>
+      <c r="C37" s="25"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>